<commit_message>
working on Champion object
</commit_message>
<xml_diff>
--- a/Documents/Digivolution plan.xlsx
+++ b/Documents/Digivolution plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="In-Training Digivolution" sheetId="4" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -430,6 +430,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,7 +799,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,46 +821,46 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>57</v>
       </c>
     </row>
@@ -870,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,134 +893,134 @@
       <c r="B1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1057,24 +1060,24 @@
       <c r="B1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6"/>
@@ -1087,11 +1090,11 @@
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="6"/>
@@ -1104,14 +1107,14 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="6"/>
@@ -1123,14 +1126,14 @@
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="6"/>
@@ -1142,17 +1145,17 @@
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="6"/>
@@ -1163,14 +1166,14 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="6"/>
@@ -1182,14 +1185,14 @@
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="6"/>
@@ -1201,11 +1204,11 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="7"/>
@@ -1218,116 +1221,116 @@
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="6"/>
@@ -1338,11 +1341,11 @@
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="6"/>
@@ -1355,11 +1358,11 @@
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="6"/>
@@ -1372,14 +1375,14 @@
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="6"/>
@@ -1391,14 +1394,14 @@
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="11" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="6"/>
@@ -1410,14 +1413,14 @@
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="6"/>
@@ -1429,14 +1432,14 @@
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="6"/>
@@ -1448,16 +1451,16 @@
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E20" s="6"/>
@@ -1469,16 +1472,16 @@
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="6"/>
@@ -1490,16 +1493,16 @@
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="6"/>
@@ -1511,16 +1514,16 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="12" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="6"/>
@@ -1532,13 +1535,13 @@
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="6"/>
@@ -1551,16 +1554,16 @@
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="6"/>
@@ -1572,16 +1575,16 @@
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="6"/>
@@ -1614,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,39 +1643,39 @@
       <c r="B1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="6"/>
@@ -1682,25 +1685,25 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="6"/>
@@ -1710,13 +1713,13 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="6"/>
@@ -1730,13 +1733,13 @@
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="6"/>
@@ -1750,13 +1753,13 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="6"/>
@@ -1770,25 +1773,25 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="6"/>
@@ -1798,22 +1801,22 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="6"/>
@@ -1824,25 +1827,25 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="6"/>
@@ -1852,19 +1855,19 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="6"/>
@@ -1876,25 +1879,25 @@
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>43</v>
       </c>
       <c r="H11" s="6"/>
@@ -1904,40 +1907,40 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="12" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>